<commit_message>
routine work on the script
</commit_message>
<xml_diff>
--- a/user_data/procedures.xlsx
+++ b/user_data/procedures.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matushev_work\Desktop\СОХРАН\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\VB\saloon_bot\user_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3F15C7D4-14E3-4639-9E25-EABE64B74220}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D9798E-8BFA-493A-9B4D-7CCF4A9A4FB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{10DDC76F-6511-457A-BFE1-435268922275}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>Процедура</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>13:00-20:00</t>
+  </si>
+  <si>
+    <t>Коррекция бровей</t>
   </si>
 </sst>
 </file>
@@ -473,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{544C202D-3401-4227-B28E-A33D49D4373D}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,6 +576,11 @@
         <v>15</v>
       </c>
     </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
wip & added procedures table update from excel
</commit_message>
<xml_diff>
--- a/user_data/procedures.xlsx
+++ b/user_data/procedures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\VB\saloon_bot\user_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D9798E-8BFA-493A-9B4D-7CCF4A9A4FB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE76D59-7C48-44ED-8757-04E273394F90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{10DDC76F-6511-457A-BFE1-435268922275}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{10DDC76F-6511-457A-BFE1-435268922275}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>Процедура</t>
   </si>
@@ -479,7 +479,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,7 +487,7 @@
     <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -579,6 +579,15 @@
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="C5">
+        <v>30</v>
+      </c>
+      <c r="I5" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>